<commit_message>
Mosfet Araştırmaları Excel'e Eklendi.
</commit_message>
<xml_diff>
--- a/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
+++ b/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onur\Desktop\ELEKTRONIK\sensored-bldc-driver\PCB\sensored-bldc-driver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onur\Desktop\ELEKTRONIK\sensored-bldc-driver\PCB\sensored-bldc-driver\Araştırmalar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB6E55F-DAFC-43FB-920B-3B8F4FDBBF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31263AA-5E1A-4F56-A775-54826BF0E5F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Filtrelenmiş Aramalar" sheetId="1" r:id="rId1"/>
     <sheet name="DC-DC Converter" sheetId="2" r:id="rId2"/>
+    <sheet name="MOSFET" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
   <si>
     <t>DC / DC Converter</t>
   </si>
@@ -179,17 +180,213 @@
   </si>
   <si>
     <t>Komponent No</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>MANUFACTURER</t>
+  </si>
+  <si>
+    <t>MANUFACTURER NO</t>
+  </si>
+  <si>
+    <t>VDS</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>RDS-ON</t>
+  </si>
+  <si>
+    <t>P30B10EL-5071</t>
+  </si>
+  <si>
+    <t>SHINDENGEN</t>
+  </si>
+  <si>
+    <t>100V</t>
+  </si>
+  <si>
+    <t>30A</t>
+  </si>
+  <si>
+    <t>24mR</t>
+  </si>
+  <si>
+    <t>IRFR3410TRLPBF</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>31A</t>
+  </si>
+  <si>
+    <t>39mR</t>
+  </si>
+  <si>
+    <t>P32B12SN-5071</t>
+  </si>
+  <si>
+    <t>120V</t>
+  </si>
+  <si>
+    <t>32A</t>
+  </si>
+  <si>
+    <t>20mR</t>
+  </si>
+  <si>
+    <t>IRF540NSTRLPBF</t>
+  </si>
+  <si>
+    <t>INFINEON</t>
+  </si>
+  <si>
+    <t>33A</t>
+  </si>
+  <si>
+    <t>44mR</t>
+  </si>
+  <si>
+    <t>IRFR540ZTRPBF</t>
+  </si>
+  <si>
+    <t>35A</t>
+  </si>
+  <si>
+    <t>22.5mR</t>
+  </si>
+  <si>
+    <t>P40B10SL-5071</t>
+  </si>
+  <si>
+    <t>40A</t>
+  </si>
+  <si>
+    <t>14.8mR</t>
+  </si>
+  <si>
+    <t>IRF1310NSTRLPBF</t>
+  </si>
+  <si>
+    <t>42A</t>
+  </si>
+  <si>
+    <t>36mR</t>
+  </si>
+  <si>
+    <t>IXTY44N10T-TRL</t>
+  </si>
+  <si>
+    <t>IXYS</t>
+  </si>
+  <si>
+    <t>44A</t>
+  </si>
+  <si>
+    <t>30mR</t>
+  </si>
+  <si>
+    <t>BSC117N08NS5ATMA1</t>
+  </si>
+  <si>
+    <t>80V</t>
+  </si>
+  <si>
+    <t>49A</t>
+  </si>
+  <si>
+    <t>9.6mR</t>
+  </si>
+  <si>
+    <t>CSD19534Q5A</t>
+  </si>
+  <si>
+    <t>50A</t>
+  </si>
+  <si>
+    <t>12.6mR</t>
+  </si>
+  <si>
+    <t>IRFR3607TRPBF</t>
+  </si>
+  <si>
+    <t>75V</t>
+  </si>
+  <si>
+    <t>56A</t>
+  </si>
+  <si>
+    <t>7.34mR</t>
+  </si>
+  <si>
+    <t>IRF3710STRLPBF</t>
+  </si>
+  <si>
+    <t>57A</t>
+  </si>
+  <si>
+    <t>23mR</t>
+  </si>
+  <si>
+    <t>UF3710L-TQ2-R</t>
+  </si>
+  <si>
+    <t>UTC</t>
+  </si>
+  <si>
+    <t>IXTA60N10T-TRL</t>
+  </si>
+  <si>
+    <t>60A</t>
+  </si>
+  <si>
+    <t>18mR</t>
+  </si>
+  <si>
+    <t>STB100N10F7</t>
+  </si>
+  <si>
+    <t>STM</t>
+  </si>
+  <si>
+    <t>80A</t>
+  </si>
+  <si>
+    <t>6.8mR</t>
+  </si>
+  <si>
+    <t>STOCK</t>
+  </si>
+  <si>
+    <t>PRICE ($)</t>
+  </si>
+  <si>
+    <t>PRICE (₺)</t>
+  </si>
+  <si>
+    <t>NOT</t>
+  </si>
+  <si>
+    <t>* Stoğa göre sıralanmıştır.</t>
+  </si>
+  <si>
+    <t>DOLLAR RATE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;₺&quot;* #,##0.00_-;\-&quot;₺&quot;* #,##0.00_-;_-&quot;₺&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="170" formatCode="_-[$₺-41F]* #,##0.00_-;\-[$₺-41F]* #,##0.00_-;_-[$₺-41F]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,18 +399,57 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -221,21 +457,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="%20 - Vurgu1" xfId="2" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ParaBirimi" xfId="1" builtinId="4"/>
   </cellStyles>
@@ -572,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F6FC7D-0BA6-4185-872A-1E67B064EE31}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,4 +1144,630 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555FC548-37F0-4793-A0A8-AFDA75852DD6}">
+  <dimension ref="B2:K23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="5"/>
+    <col min="3" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H2" s="5"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="15">
+        <v>111810</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="J4" s="17">
+        <f>I4*K4</f>
+        <v>28.509899999999998</v>
+      </c>
+      <c r="K4" s="21">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="15">
+        <v>38966</v>
+      </c>
+      <c r="I5" s="16">
+        <v>1.5194300000000001</v>
+      </c>
+      <c r="J5" s="17">
+        <f>I5*K4</f>
+        <v>51.508676999999999</v>
+      </c>
+      <c r="K5" s="21"/>
+    </row>
+    <row r="6" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="15">
+        <v>23542</v>
+      </c>
+      <c r="I6" s="16">
+        <v>1.39733</v>
+      </c>
+      <c r="J6" s="17">
+        <f>I6*K4</f>
+        <v>47.369486999999999</v>
+      </c>
+      <c r="K6" s="21"/>
+    </row>
+    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="12">
+        <v>4</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="15">
+        <v>18641</v>
+      </c>
+      <c r="I7" s="16">
+        <v>1.4985299999999999</v>
+      </c>
+      <c r="J7" s="17">
+        <f>I7*K4</f>
+        <v>50.800166999999995</v>
+      </c>
+      <c r="K7" s="21"/>
+    </row>
+    <row r="8" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="12">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="15">
+        <v>16716</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0.45140000000000002</v>
+      </c>
+      <c r="J8" s="17">
+        <f>I8*K4</f>
+        <v>15.30246</v>
+      </c>
+      <c r="K8" s="21"/>
+    </row>
+    <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="15">
+        <v>15982</v>
+      </c>
+      <c r="I9" s="16">
+        <v>1.5132699999999999</v>
+      </c>
+      <c r="J9" s="17">
+        <f>I9*K4</f>
+        <v>51.299852999999992</v>
+      </c>
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12">
+        <v>7</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" s="15">
+        <v>7868</v>
+      </c>
+      <c r="I10" s="16">
+        <v>2.8504999999999998</v>
+      </c>
+      <c r="J10" s="17">
+        <f>I10*K4</f>
+        <v>96.631949999999989</v>
+      </c>
+      <c r="K10" s="21"/>
+    </row>
+    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
+        <v>8</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="15">
+        <v>6278</v>
+      </c>
+      <c r="I11" s="16">
+        <v>0.77578999999999998</v>
+      </c>
+      <c r="J11" s="17">
+        <f>I11*K4</f>
+        <v>26.299280999999997</v>
+      </c>
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="15">
+        <v>4790</v>
+      </c>
+      <c r="I12" s="16">
+        <v>0.83133999999999997</v>
+      </c>
+      <c r="J12" s="17">
+        <f>I12*K4</f>
+        <v>28.182425999999996</v>
+      </c>
+      <c r="K12" s="21"/>
+    </row>
+    <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
+        <v>10</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="15">
+        <v>3230</v>
+      </c>
+      <c r="I13" s="16">
+        <v>0.98738999999999999</v>
+      </c>
+      <c r="J13" s="17">
+        <f>I13*K4</f>
+        <v>33.472521</v>
+      </c>
+      <c r="K13" s="21"/>
+    </row>
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="12">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="15">
+        <v>3079</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0.71955999999999998</v>
+      </c>
+      <c r="J14" s="17">
+        <f>I14*K4</f>
+        <v>24.393083999999998</v>
+      </c>
+      <c r="K14" s="21"/>
+    </row>
+    <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="12">
+        <v>12</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="15">
+        <v>2284</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0.79430999999999996</v>
+      </c>
+      <c r="J15" s="17">
+        <f>I15*K4</f>
+        <v>26.927108999999998</v>
+      </c>
+      <c r="K15" s="21"/>
+    </row>
+    <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12">
+        <v>13</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="15">
+        <v>1993</v>
+      </c>
+      <c r="I16" s="16">
+        <v>1.13927</v>
+      </c>
+      <c r="J16" s="17">
+        <f>I16*K4</f>
+        <v>38.621252999999996</v>
+      </c>
+      <c r="K16" s="21"/>
+    </row>
+    <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H17" s="15">
+        <v>1613</v>
+      </c>
+      <c r="I17" s="16">
+        <v>0.6946</v>
+      </c>
+      <c r="J17" s="17">
+        <f>I17*K4</f>
+        <v>23.546939999999999</v>
+      </c>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="15">
+        <v>72</v>
+      </c>
+      <c r="I18" s="16">
+        <v>1.6185400000000001</v>
+      </c>
+      <c r="J18" s="17">
+        <f>I18*K4</f>
+        <v>54.868506000000004</v>
+      </c>
+      <c r="K18" s="21"/>
+    </row>
+    <row r="19" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="22"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="22"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="22" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C4:I18">
+    <sortCondition descending="1" ref="H4:H18"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="K4:K18"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J4:J20">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Gate Driver Entegre Araştırması ve Bootstrap Tekniğiyle Alakalı Dökümanlar Ekledim.
</commit_message>
<xml_diff>
--- a/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
+++ b/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onur\Desktop\ELEKTRONIK\sensored-bldc-driver\PCB\sensored-bldc-driver\Araştırmalar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04CF540-0F96-4BB0-A10A-FA8199155B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29FD170-6D62-4998-BEAE-690027E8EE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC-DC Converter" sheetId="2" r:id="rId1"/>
     <sheet name="MOSFET" sheetId="3" r:id="rId2"/>
+    <sheet name="Gate Drivers" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="118">
   <si>
     <t>LMR16020PDDAR</t>
   </si>
@@ -344,6 +345,42 @@
   </si>
   <si>
     <t>OUTPUT CURRENT</t>
+  </si>
+  <si>
+    <t>IRS2005STRPBF</t>
+  </si>
+  <si>
+    <t>IR2101STRPBF</t>
+  </si>
+  <si>
+    <t>IR2106STRPBF</t>
+  </si>
+  <si>
+    <t>Vsupply</t>
+  </si>
+  <si>
+    <t>10V - 20V</t>
+  </si>
+  <si>
+    <t>DELAY</t>
+  </si>
+  <si>
+    <t>50ns</t>
+  </si>
+  <si>
+    <t>Io+ / Io-</t>
+  </si>
+  <si>
+    <t>290mA / 600mA</t>
+  </si>
+  <si>
+    <t>130mA / 270mA</t>
+  </si>
+  <si>
+    <t>200mA / 350mA</t>
+  </si>
+  <si>
+    <t>30nS</t>
   </si>
 </sst>
 </file>
@@ -493,13 +530,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -533,14 +571,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,33 +585,30 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="%20 - Vurgu1" xfId="2" builtinId="30"/>
     <cellStyle name="%40 - Vurgu1" xfId="3" builtinId="31"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ParaBirimi" xfId="1" builtinId="4"/>
+    <cellStyle name="Yüzde" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -856,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F6FC7D-0BA6-4185-872A-1E67B064EE31}">
   <dimension ref="B4:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,14 +965,14 @@
         <v>30</v>
       </c>
       <c r="I7" s="8"/>
-      <c r="J7" s="17">
+      <c r="J7" s="15">
         <v>0.99751000000000001</v>
       </c>
       <c r="K7" s="11">
         <f>J7*L7</f>
         <v>33.815588999999996</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="18">
         <v>33.9</v>
       </c>
     </row>
@@ -974,7 +1006,7 @@
         <f>J8*L7</f>
         <v>55.553624999999997</v>
       </c>
-      <c r="L8" s="20"/>
+      <c r="L8" s="19"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
@@ -1006,7 +1038,7 @@
         <f>J9*L7</f>
         <v>60.866432999999994</v>
       </c>
-      <c r="L9" s="20"/>
+      <c r="L9" s="19"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
@@ -1038,7 +1070,7 @@
         <f>J10*L7</f>
         <v>66.856562999999994</v>
       </c>
-      <c r="L10" s="20"/>
+      <c r="L10" s="19"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
@@ -1059,10 +1091,10 @@
       <c r="G11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="18"/>
+      <c r="I11" s="16"/>
       <c r="J11" s="11">
         <v>2.0135100000000001</v>
       </c>
@@ -1070,7 +1102,7 @@
         <f>J11*L7</f>
         <v>68.257988999999995</v>
       </c>
-      <c r="L11" s="20"/>
+      <c r="L11" s="19"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
@@ -1092,7 +1124,7 @@
         <f>J12*L7</f>
         <v>0</v>
       </c>
-      <c r="L12" s="20"/>
+      <c r="L12" s="19"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
@@ -1114,7 +1146,7 @@
         <f>J13*L7</f>
         <v>0</v>
       </c>
-      <c r="L13" s="20"/>
+      <c r="L13" s="19"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
@@ -1136,7 +1168,7 @@
         <f>J14*L7</f>
         <v>0</v>
       </c>
-      <c r="L14" s="20"/>
+      <c r="L14" s="19"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
@@ -1158,7 +1190,7 @@
         <f>J15*L7</f>
         <v>0</v>
       </c>
-      <c r="L15" s="20"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
@@ -1180,7 +1212,7 @@
         <f>J16*L7</f>
         <v>0</v>
       </c>
-      <c r="L16" s="20"/>
+      <c r="L16" s="19"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
@@ -1202,7 +1234,7 @@
         <f>J17*L7</f>
         <v>0</v>
       </c>
-      <c r="L17" s="20"/>
+      <c r="L17" s="19"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
@@ -1224,7 +1256,7 @@
         <f>J18*L7</f>
         <v>0</v>
       </c>
-      <c r="L18" s="20"/>
+      <c r="L18" s="19"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
@@ -1246,7 +1278,7 @@
         <f>J19*L7</f>
         <v>0</v>
       </c>
-      <c r="L19" s="20"/>
+      <c r="L19" s="19"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
@@ -1268,7 +1300,7 @@
         <f>J20*L7</f>
         <v>0</v>
       </c>
-      <c r="L20" s="20"/>
+      <c r="L20" s="19"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
@@ -1290,7 +1322,7 @@
         <f>J21*L7</f>
         <v>0</v>
       </c>
-      <c r="L21" s="20"/>
+      <c r="L21" s="19"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
@@ -1312,7 +1344,7 @@
         <f>J22*L7</f>
         <v>0</v>
       </c>
-      <c r="L22" s="20"/>
+      <c r="L22" s="19"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
@@ -1334,7 +1366,7 @@
         <f>J23*L7</f>
         <v>0</v>
       </c>
-      <c r="L23" s="20"/>
+      <c r="L23" s="19"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
@@ -1356,37 +1388,37 @@
         <f>J24*L7</f>
         <v>0</v>
       </c>
-      <c r="L24" s="21"/>
+      <c r="L24" s="20"/>
     </row>
     <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="16" t="s">
+      <c r="B30" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1427,7 +1459,7 @@
   <dimension ref="B5:K28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="K7" sqref="K7:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1540,7 @@
         <f>I7*K7</f>
         <v>28.509899999999998</v>
       </c>
-      <c r="K7" s="22">
+      <c r="K7" s="23">
         <v>33.9</v>
       </c>
     </row>
@@ -1541,7 +1573,7 @@
         <f>I8*K7</f>
         <v>51.508676999999999</v>
       </c>
-      <c r="K8" s="22"/>
+      <c r="K8" s="23"/>
     </row>
     <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
@@ -1572,7 +1604,7 @@
         <f>I9*K7</f>
         <v>47.369486999999999</v>
       </c>
-      <c r="K9" s="22"/>
+      <c r="K9" s="23"/>
     </row>
     <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
@@ -1603,7 +1635,7 @@
         <f>I10*K7</f>
         <v>50.800166999999995</v>
       </c>
-      <c r="K10" s="22"/>
+      <c r="K10" s="23"/>
     </row>
     <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
@@ -1634,7 +1666,7 @@
         <f>I11*K7</f>
         <v>15.30246</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="23"/>
     </row>
     <row r="12" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
@@ -1665,7 +1697,7 @@
         <f>I12*K7</f>
         <v>51.299852999999992</v>
       </c>
-      <c r="K12" s="22"/>
+      <c r="K12" s="23"/>
     </row>
     <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
@@ -1696,7 +1728,7 @@
         <f>I13*K7</f>
         <v>96.631949999999989</v>
       </c>
-      <c r="K13" s="22"/>
+      <c r="K13" s="23"/>
     </row>
     <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
@@ -1727,7 +1759,7 @@
         <f>I14*K7</f>
         <v>26.299280999999997</v>
       </c>
-      <c r="K14" s="22"/>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
@@ -1758,7 +1790,7 @@
         <f>I15*K7</f>
         <v>28.182425999999996</v>
       </c>
-      <c r="K15" s="22"/>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
@@ -1789,7 +1821,7 @@
         <f>I16*K7</f>
         <v>33.472521</v>
       </c>
-      <c r="K16" s="22"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
@@ -1820,7 +1852,7 @@
         <f>I17*K7</f>
         <v>24.393083999999998</v>
       </c>
-      <c r="K17" s="22"/>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
@@ -1851,7 +1883,7 @@
         <f>I18*K7</f>
         <v>26.927108999999998</v>
       </c>
-      <c r="K18" s="22"/>
+      <c r="K18" s="23"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
@@ -1882,7 +1914,7 @@
         <f>I19*K7</f>
         <v>38.621252999999996</v>
       </c>
-      <c r="K19" s="22"/>
+      <c r="K19" s="23"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
@@ -1913,7 +1945,7 @@
         <f>I20*K7</f>
         <v>23.546939999999999</v>
       </c>
-      <c r="K20" s="22"/>
+      <c r="K20" s="23"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
@@ -1944,19 +1976,14 @@
         <f>I21*K7</f>
         <v>54.868506000000004</v>
       </c>
-      <c r="K21" s="22"/>
+      <c r="K21" s="23"/>
     </row>
     <row r="22" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="30"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E23" s="5"/>
@@ -1980,32 +2007,32 @@
       <c r="K25" s="14"/>
     </row>
     <row r="27" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C7:I21">
@@ -2058,4 +2085,219 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D5EF2E-A101-471C-A7F9-2BFB391CB212}">
+  <dimension ref="B1:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="26" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="26">
+        <v>817</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.58189999999999997</v>
+      </c>
+      <c r="J7" s="4">
+        <f>I7*K7</f>
+        <v>19.726409999999998</v>
+      </c>
+      <c r="K7" s="23">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H8" s="26">
+        <v>13043</v>
+      </c>
+      <c r="I8" s="27">
+        <v>1.30196</v>
+      </c>
+      <c r="J8" s="4">
+        <f>I8*K7</f>
+        <v>44.136443999999997</v>
+      </c>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="26">
+        <v>21819</v>
+      </c>
+      <c r="I9" s="27">
+        <v>1.3387</v>
+      </c>
+      <c r="J9" s="4">
+        <f>I9*K7</f>
+        <v>45.381929999999997</v>
+      </c>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K7:K21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Gate Driver Şemasının Temelini Çizdim.
</commit_message>
<xml_diff>
--- a/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
+++ b/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onur\Desktop\ELEKTRONIK\sensored-bldc-driver\PCB\sensored-bldc-driver\Araştırmalar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29FD170-6D62-4998-BEAE-690027E8EE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C3FA47-7653-44F5-A42F-B289E989D565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC-DC Converter" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="118">
   <si>
     <t>LMR16020PDDAR</t>
   </si>
@@ -537,7 +537,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -576,6 +576,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,8 +606,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="%20 - Vurgu1" xfId="2" builtinId="30"/>
@@ -972,7 +976,7 @@
         <f>J7*L7</f>
         <v>33.815588999999996</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="22">
         <v>33.9</v>
       </c>
     </row>
@@ -1006,7 +1010,7 @@
         <f>J8*L7</f>
         <v>55.553624999999997</v>
       </c>
-      <c r="L8" s="19"/>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
@@ -1038,7 +1042,7 @@
         <f>J9*L7</f>
         <v>60.866432999999994</v>
       </c>
-      <c r="L9" s="19"/>
+      <c r="L9" s="23"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
@@ -1070,7 +1074,7 @@
         <f>J10*L7</f>
         <v>66.856562999999994</v>
       </c>
-      <c r="L10" s="19"/>
+      <c r="L10" s="23"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
@@ -1102,7 +1106,7 @@
         <f>J11*L7</f>
         <v>68.257988999999995</v>
       </c>
-      <c r="L11" s="19"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
@@ -1124,7 +1128,7 @@
         <f>J12*L7</f>
         <v>0</v>
       </c>
-      <c r="L12" s="19"/>
+      <c r="L12" s="23"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
@@ -1146,7 +1150,7 @@
         <f>J13*L7</f>
         <v>0</v>
       </c>
-      <c r="L13" s="19"/>
+      <c r="L13" s="23"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
@@ -1168,7 +1172,7 @@
         <f>J14*L7</f>
         <v>0</v>
       </c>
-      <c r="L14" s="19"/>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
@@ -1190,7 +1194,7 @@
         <f>J15*L7</f>
         <v>0</v>
       </c>
-      <c r="L15" s="19"/>
+      <c r="L15" s="23"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
@@ -1212,7 +1216,7 @@
         <f>J16*L7</f>
         <v>0</v>
       </c>
-      <c r="L16" s="19"/>
+      <c r="L16" s="23"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
@@ -1234,7 +1238,7 @@
         <f>J17*L7</f>
         <v>0</v>
       </c>
-      <c r="L17" s="19"/>
+      <c r="L17" s="23"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
@@ -1256,7 +1260,7 @@
         <f>J18*L7</f>
         <v>0</v>
       </c>
-      <c r="L18" s="19"/>
+      <c r="L18" s="23"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
@@ -1278,7 +1282,7 @@
         <f>J19*L7</f>
         <v>0</v>
       </c>
-      <c r="L19" s="19"/>
+      <c r="L19" s="23"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
@@ -1300,7 +1304,7 @@
         <f>J20*L7</f>
         <v>0</v>
       </c>
-      <c r="L20" s="19"/>
+      <c r="L20" s="23"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
@@ -1322,7 +1326,7 @@
         <f>J21*L7</f>
         <v>0</v>
       </c>
-      <c r="L21" s="19"/>
+      <c r="L21" s="23"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="7">
@@ -1344,7 +1348,7 @@
         <f>J22*L7</f>
         <v>0</v>
       </c>
-      <c r="L22" s="19"/>
+      <c r="L22" s="23"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="7">
@@ -1366,7 +1370,7 @@
         <f>J23*L7</f>
         <v>0</v>
       </c>
-      <c r="L23" s="19"/>
+      <c r="L23" s="23"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="7">
@@ -1388,37 +1392,37 @@
         <f>J24*L7</f>
         <v>0</v>
       </c>
-      <c r="L24" s="20"/>
+      <c r="L24" s="24"/>
     </row>
     <row r="30" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1458,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555FC548-37F0-4793-A0A8-AFDA75852DD6}">
   <dimension ref="B5:K28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7:K21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1540,7 +1544,7 @@
         <f>I7*K7</f>
         <v>28.509899999999998</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="27">
         <v>33.9</v>
       </c>
     </row>
@@ -1573,7 +1577,7 @@
         <f>I8*K7</f>
         <v>51.508676999999999</v>
       </c>
-      <c r="K8" s="23"/>
+      <c r="K8" s="27"/>
     </row>
     <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
@@ -1604,7 +1608,7 @@
         <f>I9*K7</f>
         <v>47.369486999999999</v>
       </c>
-      <c r="K9" s="23"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
@@ -1635,7 +1639,7 @@
         <f>I10*K7</f>
         <v>50.800166999999995</v>
       </c>
-      <c r="K10" s="23"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
@@ -1666,7 +1670,7 @@
         <f>I11*K7</f>
         <v>15.30246</v>
       </c>
-      <c r="K11" s="23"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
@@ -1697,7 +1701,7 @@
         <f>I12*K7</f>
         <v>51.299852999999992</v>
       </c>
-      <c r="K12" s="23"/>
+      <c r="K12" s="27"/>
     </row>
     <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
@@ -1728,7 +1732,7 @@
         <f>I13*K7</f>
         <v>96.631949999999989</v>
       </c>
-      <c r="K13" s="23"/>
+      <c r="K13" s="27"/>
     </row>
     <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
@@ -1759,7 +1763,7 @@
         <f>I14*K7</f>
         <v>26.299280999999997</v>
       </c>
-      <c r="K14" s="23"/>
+      <c r="K14" s="27"/>
     </row>
     <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
@@ -1790,7 +1794,7 @@
         <f>I15*K7</f>
         <v>28.182425999999996</v>
       </c>
-      <c r="K15" s="23"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
@@ -1821,7 +1825,7 @@
         <f>I16*K7</f>
         <v>33.472521</v>
       </c>
-      <c r="K16" s="23"/>
+      <c r="K16" s="27"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
@@ -1852,7 +1856,7 @@
         <f>I17*K7</f>
         <v>24.393083999999998</v>
       </c>
-      <c r="K17" s="23"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
@@ -1883,7 +1887,7 @@
         <f>I18*K7</f>
         <v>26.927108999999998</v>
       </c>
-      <c r="K18" s="23"/>
+      <c r="K18" s="27"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="7">
@@ -1914,7 +1918,7 @@
         <f>I19*K7</f>
         <v>38.621252999999996</v>
       </c>
-      <c r="K19" s="23"/>
+      <c r="K19" s="27"/>
     </row>
     <row r="20" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7">
@@ -1945,7 +1949,7 @@
         <f>I20*K7</f>
         <v>23.546939999999999</v>
       </c>
-      <c r="K20" s="23"/>
+      <c r="K20" s="27"/>
     </row>
     <row r="21" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7">
@@ -1976,7 +1980,7 @@
         <f>I21*K7</f>
         <v>54.868506000000004</v>
       </c>
-      <c r="K21" s="23"/>
+      <c r="K21" s="27"/>
     </row>
     <row r="22" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E22" s="5"/>
@@ -2007,32 +2011,32 @@
       <c r="K25" s="14"/>
     </row>
     <row r="27" spans="2:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C7:I21">
@@ -2091,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D5EF2E-A101-471C-A7F9-2BFB391CB212}">
   <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2100,7 +2104,7 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="26" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="18" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="4" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
@@ -2163,141 +2167,192 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C7" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F7" t="s">
-        <v>114</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="H7" s="20">
+        <v>21819</v>
+      </c>
+      <c r="I7" s="21">
+        <v>1.3387</v>
+      </c>
+      <c r="J7" s="12">
+        <f>I7*K7</f>
+        <v>45.381929999999997</v>
+      </c>
+      <c r="K7" s="27">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7">
+        <v>2</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H7" s="26">
-        <v>817</v>
-      </c>
-      <c r="I7" s="27">
-        <v>0.58189999999999997</v>
-      </c>
-      <c r="J7" s="4">
-        <f>I7*K7</f>
-        <v>19.726409999999998</v>
-      </c>
-      <c r="K7" s="23">
-        <v>33.9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>110</v>
-      </c>
-      <c r="F8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="26">
+      <c r="H8" s="20">
         <v>13043</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="21">
         <v>1.30196</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="12">
         <f>I8*K7</f>
         <v>44.136443999999997</v>
       </c>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="K8" s="27"/>
+    </row>
+    <row r="9" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
         <v>3</v>
       </c>
-      <c r="C9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="F9" t="s">
-        <v>116</v>
-      </c>
-      <c r="G9" t="s">
-        <v>117</v>
-      </c>
-      <c r="H9" s="26">
-        <v>21819</v>
-      </c>
-      <c r="I9" s="27">
-        <v>1.3387</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="F9" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="20">
+        <v>817</v>
+      </c>
+      <c r="I9" s="21">
+        <v>0.58189999999999997</v>
+      </c>
+      <c r="J9" s="12">
         <f>I9*K7</f>
-        <v>45.381929999999997</v>
-      </c>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K10" s="23"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K13" s="23"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K14" s="23"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K15" s="23"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K17" s="23"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K18" s="23"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K19" s="23"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K20" s="23"/>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K21" s="23"/>
+        <v>19.726409999999998</v>
+      </c>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="19"/>
+    </row>
+    <row r="11" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="19"/>
+    </row>
+    <row r="12" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="19"/>
+    </row>
+    <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="19"/>
+    </row>
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="19"/>
+    </row>
+    <row r="15" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="19"/>
+    </row>
+    <row r="18" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="19"/>
+    </row>
+    <row r="19" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="19"/>
+    </row>
+    <row r="21" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="K7:K21"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C7:J9">
+    <sortCondition descending="1" ref="H7:H9"/>
+  </sortState>
+  <mergeCells count="3">
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="B15:K15"/>
+    <mergeCell ref="B16:K16"/>
   </mergeCells>
+  <conditionalFormatting sqref="I7:I9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7:J9">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Yeni bir döküman ekledim, Çevirisi yapılacak.
</commit_message>
<xml_diff>
--- a/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
+++ b/PCB/sensored-bldc-driver/Araştırmalar/Komponenet Araştırmaları.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Onur\Desktop\ELEKTRONIK\sensored-bldc-driver\PCB\sensored-bldc-driver\Araştırmalar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C95415C-FAAD-4746-A4A3-D155C868909A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABA9F1A-D38B-4575-AB82-304CAEBC975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DC-DC Converter" sheetId="2" r:id="rId1"/>
@@ -1462,7 +1462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555FC548-37F0-4793-A0A8-AFDA75852DD6}">
   <dimension ref="B5:K28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2095,7 +2095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D5EF2E-A101-471C-A7F9-2BFB391CB212}">
   <dimension ref="B1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>